<commit_message>
Update de la liste de matériel
</commit_message>
<xml_diff>
--- a/Partie_LucasCannizzaro/listeMateriels.xlsx
+++ b/Partie_LucasCannizzaro/listeMateriels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guest2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillaume\Desktop\Projet BTS\Partie_LucasCannizzaro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31199BCC-1FFF-441A-B8C8-F23485611C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2769FF2-25F7-4465-8D4A-CCC7AA9A3518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{64B69FF7-E77F-4A43-A005-7164FA6CD9A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{64B69FF7-E77F-4A43-A005-7164FA6CD9A6}"/>
   </bookViews>
   <sheets>
     <sheet name="CEREMA" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Matèreils prêtés par CEREMA</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>Bouton poussoir</t>
+  </si>
+  <si>
+    <t>Matériel fourni par CEREMA</t>
+  </si>
+  <si>
+    <t>DFROBOT DFR0478</t>
+  </si>
+  <si>
+    <t>Laser CG 03                                        (3 et 4)</t>
   </si>
 </sst>
 </file>
@@ -461,40 +470,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C40C6AE-7E7E-427B-83BE-80586A346425}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.85546875" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3">
         <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>